<commit_message>
agregando la columna de nombre en ascensores3
</commit_message>
<xml_diff>
--- a/estacionestado.xlsx
+++ b/estacionestado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CONFIABILIDAD\Documents\graficos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CONFIABILIDAD\Documents\ascensorestel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8D54FA-AD51-44A3-AE41-96CC5C7F9E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72BF20D-36FF-4FE1-9B5E-12405F4188A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="2445" windowWidth="21600" windowHeight="11385" xr2:uid="{9B9B22DD-05ED-49DA-851E-9156B7E4F05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B9B22DD-05ED-49DA-851E-9156B7E4F05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>codigo_asc</t>
   </si>
   <si>
-    <t>Estacion</t>
-  </si>
-  <si>
     <t>linea</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>Escalera Eléctrica</t>
+  </si>
+  <si>
+    <t>nombre</t>
   </si>
 </sst>
 </file>
@@ -846,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755CD635-95C9-408C-9A43-BEF1945792F8}">
   <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,13 +857,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D1" s="27" t="s">
         <v>65</v>
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -971,7 +971,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1317,7 +1317,7 @@
     </row>
     <row r="28" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>2</v>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="29" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>2</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="58" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>2</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="59" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>2</v>
@@ -1861,7 +1861,7 @@
     </row>
     <row r="60" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>2</v>

</xml_diff>